<commit_message>
replace range with rssi adjacencie caldulation
</commit_message>
<xml_diff>
--- a/son_input.xlsx
+++ b/son_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklaskluge/Desktop/son/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F54A120-F540-E044-8115-C8B79C4B17E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5681009-4B7C-B947-9688-6541A12EAB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="67">
   <si>
     <t>pos_x</t>
   </si>
@@ -51,9 +51,6 @@
     <t>initial_cells</t>
   </si>
   <si>
-    <t>range</t>
-  </si>
-  <si>
     <t>bs_1</t>
   </si>
   <si>
@@ -168,9 +165,6 @@
     <t>noise</t>
   </si>
   <si>
-    <t>interference</t>
-  </si>
-  <si>
     <t>shadow_component</t>
   </si>
   <si>
@@ -226,6 +220,9 @@
   </si>
   <si>
     <t>cell_16</t>
+  </si>
+  <si>
+    <t>wave_length</t>
   </si>
 </sst>
 </file>
@@ -606,7 +603,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -645,12 +642,12 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>11</v>
@@ -659,10 +656,10 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2">
         <v>4</v>
@@ -677,15 +674,15 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2">
-        <v>13</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>21</v>
@@ -694,10 +691,10 @@
         <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F3">
         <v>4</v>
@@ -712,15 +709,15 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K3">
-        <v>13</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>39</v>
@@ -729,10 +726,10 @@
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4">
         <v>4</v>
@@ -747,15 +744,15 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K4">
-        <v>13</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>38</v>
@@ -764,10 +761,10 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -782,15 +779,15 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K5">
-        <v>13</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>20</v>
@@ -799,10 +796,10 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>1.5</v>
@@ -817,15 +814,15 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K6">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -834,10 +831,10 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <v>1.5</v>
@@ -852,15 +849,15 @@
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K7">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8">
         <v>14</v>
@@ -869,10 +866,10 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <v>1.5</v>
@@ -887,15 +884,15 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K8">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>9</v>
@@ -904,10 +901,10 @@
         <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <v>1.5</v>
@@ -922,15 +919,15 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K9">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>19</v>
@@ -939,10 +936,10 @@
         <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>1.5</v>
@@ -957,15 +954,15 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K10">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11">
         <v>27</v>
@@ -974,10 +971,10 @@
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>1.5</v>
@@ -992,15 +989,15 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K11">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12">
         <v>35</v>
@@ -1009,10 +1006,10 @@
         <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>1.5</v>
@@ -1027,15 +1024,15 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K12">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13">
         <v>42</v>
@@ -1044,10 +1041,10 @@
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <v>1.5</v>
@@ -1062,15 +1059,15 @@
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K13">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14">
         <v>51</v>
@@ -1079,10 +1076,10 @@
         <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <v>1.5</v>
@@ -1097,15 +1094,15 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K14">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15">
         <v>38</v>
@@ -1114,10 +1111,10 @@
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F15">
         <v>1.5</v>
@@ -1132,15 +1129,15 @@
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K15">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16">
         <v>26</v>
@@ -1149,10 +1146,10 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <v>1.5</v>
@@ -1167,15 +1164,15 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K16">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17">
         <v>39</v>
@@ -1184,10 +1181,10 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F17">
         <v>1.5</v>
@@ -1202,15 +1199,15 @@
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K17">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18">
         <v>47</v>
@@ -1219,10 +1216,10 @@
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F18">
         <v>1.5</v>
@@ -1237,10 +1234,10 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K18">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -1254,15 +1251,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1270,27 +1270,24 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>49</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>51</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -1307,19 +1304,16 @@
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -1336,19 +1330,16 @@
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>52</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>54</v>
       </c>
       <c r="B4">
         <v>21</v>
@@ -1365,19 +1356,16 @@
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I4">
+      <c r="G4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5">
         <v>8</v>
@@ -1394,19 +1382,16 @@
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>52</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -1423,19 +1408,16 @@
       <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7">
         <v>13</v>
@@ -1452,19 +1434,16 @@
       <c r="F7">
         <v>0</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7" t="s">
-        <v>52</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B8">
         <v>25</v>
@@ -1481,19 +1460,16 @@
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
-        <v>52</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B9">
         <v>32</v>
@@ -1510,19 +1486,16 @@
       <c r="F9">
         <v>0</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9" t="s">
-        <v>52</v>
-      </c>
-      <c r="I9">
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B10">
         <v>42</v>
@@ -1539,19 +1512,16 @@
       <c r="F10">
         <v>0</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>52</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B11">
         <v>51</v>
@@ -1568,19 +1538,16 @@
       <c r="F11">
         <v>0</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11" t="s">
-        <v>52</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B12">
         <v>42</v>
@@ -1597,19 +1564,16 @@
       <c r="F12">
         <v>0</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B13">
         <v>49</v>
@@ -1626,19 +1590,16 @@
       <c r="F13">
         <v>0</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
-        <v>52</v>
-      </c>
-      <c r="I13">
+      <c r="G13" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B14">
         <v>31</v>
@@ -1655,19 +1616,16 @@
       <c r="F14">
         <v>0</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14" t="s">
-        <v>52</v>
-      </c>
-      <c r="I14">
+      <c r="G14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B15">
         <v>44</v>
@@ -1684,19 +1642,16 @@
       <c r="F15">
         <v>0</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15" t="s">
-        <v>52</v>
-      </c>
-      <c r="I15">
+      <c r="G15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B16">
         <v>35</v>
@@ -1713,19 +1668,16 @@
       <c r="F16">
         <v>0</v>
       </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16" t="s">
-        <v>52</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -1742,19 +1694,16 @@
       <c r="F17">
         <v>0</v>
       </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17" t="s">
-        <v>52</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18">
         <v>45</v>
@@ -1771,19 +1720,16 @@
       <c r="F18">
         <v>0</v>
       </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
-        <v>52</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19">
         <v>47</v>
@@ -1800,19 +1746,16 @@
       <c r="F19">
         <v>0</v>
       </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19" t="s">
-        <v>52</v>
-      </c>
-      <c r="I19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20">
         <v>44</v>
@@ -1829,19 +1772,16 @@
       <c r="F20">
         <v>0</v>
       </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20" t="s">
-        <v>52</v>
-      </c>
-      <c r="I20">
+      <c r="G20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H20">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21">
         <v>39</v>
@@ -1858,19 +1798,16 @@
       <c r="F21">
         <v>0</v>
       </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21" t="s">
-        <v>52</v>
-      </c>
-      <c r="I21">
+      <c r="G21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22">
         <v>39</v>
@@ -1887,19 +1824,16 @@
       <c r="F22">
         <v>0</v>
       </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22" t="s">
-        <v>52</v>
-      </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23">
         <v>16</v>
@@ -1916,19 +1850,16 @@
       <c r="F23">
         <v>0</v>
       </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23" t="s">
-        <v>52</v>
-      </c>
-      <c r="I23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24">
         <v>25</v>
@@ -1945,19 +1876,16 @@
       <c r="F24">
         <v>0</v>
       </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24" t="s">
-        <v>52</v>
-      </c>
-      <c r="I24">
+      <c r="G24" t="s">
+        <v>50</v>
+      </c>
+      <c r="H24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25">
         <v>27</v>
@@ -1974,19 +1902,16 @@
       <c r="F25">
         <v>0</v>
       </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25" t="s">
-        <v>52</v>
-      </c>
-      <c r="I25">
+      <c r="G25" t="s">
+        <v>50</v>
+      </c>
+      <c r="H25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26">
         <v>6</v>
@@ -2003,19 +1928,16 @@
       <c r="F26">
         <v>0</v>
       </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26" t="s">
-        <v>52</v>
-      </c>
-      <c r="I26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27">
         <v>13</v>
@@ -2032,19 +1954,16 @@
       <c r="F27">
         <v>0</v>
       </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27" t="s">
-        <v>52</v>
-      </c>
-      <c r="I27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>12</v>
@@ -2061,19 +1980,16 @@
       <c r="F28">
         <v>0</v>
       </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28" t="s">
-        <v>52</v>
-      </c>
-      <c r="I28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>50</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29">
         <v>18</v>
@@ -2090,19 +2006,16 @@
       <c r="F29">
         <v>0</v>
       </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29" t="s">
-        <v>52</v>
-      </c>
-      <c r="I29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G29" t="s">
+        <v>50</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30">
         <v>31</v>
@@ -2119,13 +2032,10 @@
       <c r="F30">
         <v>0</v>
       </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30" t="s">
-        <v>52</v>
-      </c>
-      <c r="I30">
+      <c r="G30" t="s">
+        <v>50</v>
+      </c>
+      <c r="H30">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changing to json format, adjusting objectives
</commit_message>
<xml_diff>
--- a/son_input.xlsx
+++ b/son_input.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklaskluge/Desktop/son/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5681009-4B7C-B947-9688-6541A12EAB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C60CAA6-6F99-7844-9CF3-833E36437347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baseStations" sheetId="1" r:id="rId1"/>
-    <sheet name="cells" sheetId="2" r:id="rId2"/>
-    <sheet name="traffic_profiles" sheetId="4" r:id="rId3"/>
+    <sheet name="users" sheetId="2" r:id="rId2"/>
+    <sheet name="wf_htf_tdf_bsn" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="77">
   <si>
     <t>pos_x</t>
   </si>
@@ -42,7 +42,7 @@
     <t>standby_power</t>
   </si>
   <si>
-    <t>capacity</t>
+    <t>antennas</t>
   </si>
   <si>
     <t>frequency</t>
@@ -51,6 +51,12 @@
     <t>initial_cells</t>
   </si>
   <si>
+    <t>wave_length</t>
+  </si>
+  <si>
+    <t>channel_bandwidth</t>
+  </si>
+  <si>
     <t>bs_1</t>
   </si>
   <si>
@@ -159,18 +165,12 @@
     <t>cell_19</t>
   </si>
   <si>
-    <t>max_traffic</t>
-  </si>
-  <si>
     <t>noise</t>
   </si>
   <si>
     <t>shadow_component</t>
   </si>
   <si>
-    <t>traffic_profile_id</t>
-  </si>
-  <si>
     <t>cell_1</t>
   </si>
   <si>
@@ -222,17 +222,53 @@
     <t>cell_16</t>
   </si>
   <si>
-    <t>wave_length</t>
+    <t>10</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>0100</t>
+  </si>
+  <si>
+    <t>01000</t>
+  </si>
+  <si>
+    <t>00001</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>010</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -258,9 +294,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,9 +648,11 @@
     <col min="6" max="6" width="17.1640625" customWidth="1"/>
     <col min="7" max="7" width="22.83203125" customWidth="1"/>
     <col min="10" max="10" width="28.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -642,12 +681,15 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>11</v>
@@ -656,7 +698,7 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>4</v>
@@ -674,15 +716,18 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="K2">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>21</v>
@@ -691,7 +736,7 @@
         <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -709,15 +754,18 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="K3">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>39</v>
@@ -726,7 +774,7 @@
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -744,15 +792,18 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K4">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>38</v>
@@ -761,7 +812,7 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -779,15 +830,18 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K5">
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <v>20</v>
@@ -796,7 +850,7 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -814,15 +868,18 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K6">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -831,7 +888,7 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -849,15 +906,18 @@
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K7">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>14</v>
@@ -866,7 +926,7 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -884,15 +944,18 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K8">
         <v>80</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B9">
         <v>9</v>
@@ -901,7 +964,7 @@
         <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -919,15 +982,18 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="K9">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B10">
         <v>19</v>
@@ -936,7 +1002,7 @@
         <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -954,15 +1020,18 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K10">
         <v>80</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B11">
         <v>27</v>
@@ -971,7 +1040,7 @@
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -989,15 +1058,18 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K11">
         <v>80</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B12">
         <v>35</v>
@@ -1006,7 +1078,7 @@
         <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -1024,15 +1096,18 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K12">
         <v>80</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B13">
         <v>42</v>
@@ -1041,7 +1116,7 @@
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1059,15 +1134,18 @@
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K13">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B14">
         <v>51</v>
@@ -1076,7 +1154,7 @@
         <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1094,15 +1172,18 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K14">
         <v>80</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B15">
         <v>38</v>
@@ -1111,7 +1192,7 @@
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1129,15 +1210,18 @@
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K15">
         <v>80</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B16">
         <v>26</v>
@@ -1146,7 +1230,7 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1164,15 +1248,18 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K16">
         <v>80</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B17">
         <v>39</v>
@@ -1181,7 +1268,7 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1199,15 +1286,18 @@
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K17">
         <v>80</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B18">
         <v>47</v>
@@ -1216,7 +1306,7 @@
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1234,13 +1324,16 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K18">
         <v>80</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
@@ -1251,18 +1344,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1270,22 +1364,16 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1296,22 +1384,16 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="F2" t="s">
         <v>50</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -1322,22 +1404,16 @@
         <v>12</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="F3" t="s">
         <v>50</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -1348,22 +1424,16 @@
         <v>20</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="F4" t="s">
         <v>50</v>
       </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -1374,22 +1444,16 @@
         <v>19</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="F5" t="s">
         <v>50</v>
       </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -1400,22 +1464,16 @@
         <v>27</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="F6" t="s">
         <v>50</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1426,22 +1484,16 @@
         <v>32</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="F7" t="s">
         <v>50</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1452,22 +1504,16 @@
         <v>32</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="F8" t="s">
         <v>50</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -1478,22 +1524,16 @@
         <v>26</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="F9" t="s">
         <v>50</v>
       </c>
-      <c r="H9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -1504,22 +1544,16 @@
         <v>34</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="F10" t="s">
         <v>50</v>
       </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -1530,22 +1564,16 @@
         <v>25</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="F11" t="s">
         <v>50</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1556,22 +1584,16 @@
         <v>19</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="F12" t="s">
         <v>50</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -1582,22 +1604,16 @@
         <v>12</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="F13" t="s">
         <v>50</v>
       </c>
-      <c r="H13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -1608,22 +1624,16 @@
         <v>17</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="F14" t="s">
         <v>50</v>
       </c>
-      <c r="H14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -1634,22 +1644,16 @@
         <v>6</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="F15" t="s">
         <v>50</v>
       </c>
-      <c r="H15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -1660,22 +1664,16 @@
         <v>6</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="F16" t="s">
         <v>50</v>
       </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -1686,24 +1684,18 @@
         <v>13</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="F17" t="s">
         <v>50</v>
       </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B18">
         <v>45</v>
@@ -1712,24 +1704,18 @@
         <v>29</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="F18" t="s">
         <v>50</v>
       </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B19">
         <v>47</v>
@@ -1738,24 +1724,18 @@
         <v>27</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="F19" t="s">
         <v>50</v>
       </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B20">
         <v>44</v>
@@ -1764,24 +1744,18 @@
         <v>10</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="F20" t="s">
         <v>50</v>
       </c>
-      <c r="H20">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B21">
         <v>39</v>
@@ -1790,24 +1764,18 @@
         <v>23</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="F21" t="s">
         <v>50</v>
       </c>
-      <c r="H21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B22">
         <v>39</v>
@@ -1816,24 +1784,18 @@
         <v>1</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="F22" t="s">
         <v>50</v>
       </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>16</v>
@@ -1842,24 +1804,18 @@
         <v>3</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="F23" t="s">
         <v>50</v>
       </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B24">
         <v>25</v>
@@ -1868,24 +1824,18 @@
         <v>17</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="F24" t="s">
         <v>50</v>
       </c>
-      <c r="H24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B25">
         <v>27</v>
@@ -1894,24 +1844,18 @@
         <v>20</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="F25" t="s">
         <v>50</v>
       </c>
-      <c r="H25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>6</v>
@@ -1920,24 +1864,18 @@
         <v>8</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="F26" t="s">
         <v>50</v>
       </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B27">
         <v>13</v>
@@ -1946,24 +1884,18 @@
         <v>17</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="F27" t="s">
         <v>50</v>
       </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B28">
         <v>12</v>
@@ -1972,24 +1904,18 @@
         <v>29</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="F28" t="s">
         <v>50</v>
       </c>
-      <c r="H28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B29">
         <v>18</v>
@@ -1998,24 +1924,18 @@
         <v>34</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29" t="s">
+      <c r="F29" t="s">
         <v>50</v>
       </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B30">
         <v>31</v>
@@ -2024,19 +1944,13 @@
         <v>31</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="F30" t="s">
         <v>50</v>
-      </c>
-      <c r="H30">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2045,438 +1959,1085 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AC12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0.2</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>0.2</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C4">
-        <v>0.01</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>0.01</v>
-      </c>
-      <c r="C5">
-        <v>0.05</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>0.12</v>
-      </c>
-      <c r="C6">
-        <v>0.1</v>
-      </c>
-      <c r="D6">
-        <v>0.1</v>
-      </c>
-      <c r="E6">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>0.5</v>
-      </c>
-      <c r="C7">
-        <v>0.3</v>
-      </c>
-      <c r="D7">
-        <v>0.3</v>
-      </c>
-      <c r="E7">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>0.7</v>
-      </c>
-      <c r="C8">
-        <v>0.7</v>
-      </c>
-      <c r="D8">
-        <v>0.3</v>
-      </c>
-      <c r="E8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>0.7</v>
-      </c>
-      <c r="C9">
-        <v>0.8</v>
-      </c>
-      <c r="D9">
-        <v>0.4</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>0.8</v>
-      </c>
-      <c r="C10">
-        <v>0.9</v>
-      </c>
-      <c r="D10">
-        <v>0.4</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>0.6</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>0.6</v>
-      </c>
-      <c r="E11">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>0.5</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>0.4</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>0.5</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>0.6</v>
-      </c>
-      <c r="C15">
-        <v>0.8</v>
-      </c>
-      <c r="D15">
-        <v>0.4</v>
-      </c>
-      <c r="E15">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>0.8</v>
-      </c>
-      <c r="C16">
-        <v>0.6</v>
-      </c>
-      <c r="D16">
-        <v>0.3</v>
-      </c>
-      <c r="E16">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>0.5</v>
-      </c>
-      <c r="D17">
-        <v>0.2</v>
-      </c>
-      <c r="E17">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>0.3</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>0.2</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>0.1</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>0.9</v>
-      </c>
-      <c r="C21">
-        <v>0.05</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>0.8</v>
-      </c>
-      <c r="C22">
-        <v>0.02</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>0.8</v>
-      </c>
-      <c r="C23">
-        <v>0.02</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>0.6</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>0.35</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC7" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC8" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC9" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC11" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC12" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>